<commit_message>
Feat: GRASP now supports constant effectors/inhibitors/activators
This was done by not hardcoding constant metabolites as
ones in the kinetic function, and instead have them as
 variables whose values are set to ones.
</commit_message>
<xml_diff>
--- a/matlab_code/tests/patternFxns/testFiles/toy_model1_test.xlsx
+++ b/matlab_code/tests/patternFxns/testFiles/toy_model1_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,324 +32,324 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="106">
-  <si>
-    <t>General Reaction and Sampling Platform (GRASP)</t>
-  </si>
-  <si>
-    <t>Unnamed: 1</t>
-  </si>
-  <si>
-    <t>Model name</t>
-  </si>
-  <si>
-    <t>toy_model1</t>
-  </si>
-  <si>
-    <t>Sampling mode (ORACLE, rejection, rejectionSMC, SMC, MCMC-SMC)</t>
-  </si>
-  <si>
-    <t>ORACLE</t>
-  </si>
-  <si>
-    <t>NLP solver (NLOPT, OPTI, FMINCON (default))</t>
-  </si>
-  <si>
-    <t>FMINCON</t>
-  </si>
-  <si>
-    <t>Number of exp. conditions (excluding reference state)</t>
-  </si>
-  <si>
-    <t>Number of model structures</t>
-  </si>
-  <si>
-    <t>Number of particles</t>
-  </si>
-  <si>
-    <t>Parallel mode (ON = 1; OFF = 0)</t>
-  </si>
-  <si>
-    <t>Number of cores (ignored if Parallel mode disabled)</t>
-  </si>
-  <si>
-    <t>Percentile of alive particles for SMC (e.g., 20, 50, etc.) (only needed for rejectionSMC, SMC, MCMC-SMC)</t>
-  </si>
-  <si>
-    <t>Compute robust fluxes (ON = 1; OFF = 0)</t>
-  </si>
-  <si>
-    <t>Compute thermodynamics (ON = 1; OFF = 0)</t>
-  </si>
-  <si>
-    <t>Inicial tolerance (OPTIONAL)</t>
-  </si>
-  <si>
-    <t>Final tolerance (in the case of ORACLE, set to 1)</t>
-  </si>
-  <si>
-    <t>rxn ID</t>
-  </si>
-  <si>
-    <t>m1</t>
-  </si>
-  <si>
-    <t>m2</t>
-  </si>
-  <si>
-    <t>m3</t>
-  </si>
-  <si>
-    <t>m4</t>
-  </si>
-  <si>
-    <t>m5</t>
-  </si>
-  <si>
-    <t>m6</t>
-  </si>
-  <si>
-    <t>m7</t>
-  </si>
-  <si>
-    <t>m8</t>
-  </si>
-  <si>
-    <t>m9</t>
-  </si>
-  <si>
-    <t>m10</t>
-  </si>
-  <si>
-    <t>m11</t>
-  </si>
-  <si>
-    <t>m12</t>
-  </si>
-  <si>
-    <t>m13</t>
-  </si>
-  <si>
-    <t>m14</t>
-  </si>
-  <si>
-    <t>m15</t>
-  </si>
-  <si>
-    <t>m16</t>
-  </si>
-  <si>
-    <t>m17</t>
-  </si>
-  <si>
-    <t>m18</t>
-  </si>
-  <si>
-    <t>m19</t>
-  </si>
-  <si>
-    <t>m20</t>
-  </si>
-  <si>
-    <t>r1</t>
-  </si>
-  <si>
-    <t>r2</t>
-  </si>
-  <si>
-    <t>r3</t>
-  </si>
-  <si>
-    <t>r4</t>
-  </si>
-  <si>
-    <t>r5</t>
-  </si>
-  <si>
-    <t>r6</t>
-  </si>
-  <si>
-    <t>r7</t>
-  </si>
-  <si>
-    <t>r8</t>
-  </si>
-  <si>
-    <t>r9</t>
-  </si>
-  <si>
-    <t>r10</t>
-  </si>
-  <si>
-    <t>r11</t>
-  </si>
-  <si>
-    <t>r12</t>
-  </si>
-  <si>
-    <t>r13</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Metabolite name</t>
-  </si>
-  <si>
-    <t>balanced?</t>
-  </si>
-  <si>
-    <t>active?</t>
-  </si>
-  <si>
-    <t>fixed?</t>
-  </si>
-  <si>
-    <t>measured?</t>
-  </si>
-  <si>
-    <t>reaction name</t>
-  </si>
-  <si>
-    <t>transportRxn?</t>
-  </si>
-  <si>
-    <t>modelled?</t>
-  </si>
-  <si>
-    <t>isoenzymes</t>
-  </si>
-  <si>
-    <t>met</t>
-  </si>
-  <si>
-    <t>rxn</t>
-  </si>
-  <si>
-    <t>∆Gr'_min (kJ/mol)</t>
-  </si>
-  <si>
-    <t>∆Gr'_max (kJ/mol)</t>
-  </si>
-  <si>
-    <t>min (M)</t>
-  </si>
-  <si>
-    <t>max (M)</t>
-  </si>
-  <si>
-    <t>Fluxes (umol/gCDW/h)</t>
-  </si>
-  <si>
-    <t>vref_mean</t>
-  </si>
-  <si>
-    <t>vref_std</t>
-  </si>
-  <si>
-    <t>enzyme/rxn</t>
-  </si>
-  <si>
-    <t>MBo10_LB2</t>
-  </si>
-  <si>
-    <t>MBo10_meas2</t>
-  </si>
-  <si>
-    <t>MBo10_UB2</t>
-  </si>
-  <si>
-    <t>MBo10_LB2 (M)</t>
-  </si>
-  <si>
-    <t>MBo10_UB2 (M)</t>
-  </si>
-  <si>
-    <t>reaction ID</t>
-  </si>
-  <si>
-    <t>kinetic mechanism</t>
-  </si>
-  <si>
-    <t>substrate order</t>
-  </si>
-  <si>
-    <t>product order</t>
-  </si>
-  <si>
-    <t>promiscuous</t>
-  </si>
-  <si>
-    <t>inhibitors</t>
-  </si>
-  <si>
-    <t>activators</t>
-  </si>
-  <si>
-    <t>negative effector</t>
-  </si>
-  <si>
-    <t>positive effector</t>
-  </si>
-  <si>
-    <t>allosteric</t>
-  </si>
-  <si>
-    <t>subunits</t>
-  </si>
-  <si>
-    <t>comments</t>
-  </si>
-  <si>
-    <t>substrateInhibOrderedBiBi</t>
-  </si>
-  <si>
-    <t>m3 m6</t>
-  </si>
-  <si>
-    <t>m5 m14</t>
-  </si>
-  <si>
-    <t>UniUniPromiscuous</t>
-  </si>
-  <si>
-    <t>m5 m6</t>
-  </si>
-  <si>
-    <t>m7 m10</t>
-  </si>
-  <si>
-    <t>r2 r5</t>
-  </si>
-  <si>
-    <t>OrdPromiscCompInhibIndep</t>
-  </si>
-  <si>
-    <t>m1 m7 m1 m10</t>
-  </si>
-  <si>
-    <t>m8 m11 m12 m12</t>
-  </si>
-  <si>
-    <t>r3 r6</t>
-  </si>
-  <si>
-    <t>randomBiBi2</t>
-  </si>
-  <si>
-    <t>m2 m8 </t>
-  </si>
-  <si>
-    <t>m9 m13</t>
-  </si>
-  <si>
-    <t>massAction</t>
-  </si>
-  <si>
-    <t>diffusion</t>
-  </si>
-  <si>
-    <t>fixedExchange</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="106">
+  <si>
+    <t xml:space="preserve">General Reaction and Sampling Platform (GRASP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unnamed: 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toy_model1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sampling mode (ORACLE, rejection, rejectionSMC, SMC, MCMC-SMC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORACLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLP solver (NLOPT, OPTI, FMINCON (default))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FMINCON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of exp. conditions (excluding reference state)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of model structures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of particles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parallel mode (ON = 1; OFF = 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of cores (ignored if Parallel mode disabled)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentile of alive particles for SMC (e.g., 20, 50, etc.) (only needed for rejectionSMC, SMC, MCMC-SMC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compute robust fluxes (ON = 1; OFF = 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compute thermodynamics (ON = 1; OFF = 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inicial tolerance (OPTIONAL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final tolerance (in the case of ORACLE, set to 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rxn ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metabolite name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">balanced?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">active?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fixed?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">measured?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transportRxn?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modelled?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isoenzymes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">met</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rxn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">∆Gr'_min (kJ/mol)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">∆Gr'_max (kJ/mol)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min (M)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max (M)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fluxes (umol/gCDW/h)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vref_mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vref_std</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enzyme/rxn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBo10_LB2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBo10_meas2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBo10_UB2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBo10_LB2 (M)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBo10_UB2 (M)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kinetic mechanism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">substrate order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">promiscuous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inhibitors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">negative effector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">positive effector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allosteric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subunits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">substrateInhibOrderedBiBi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m3 m6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m5 m14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UniUniPromiscuous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m5 m6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m7 m10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r2 r5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OrdPromiscCompInhibIndep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m1 m7 m1 m10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m8 m11 m12 m12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r3 r6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">randomBiBi2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m2 m8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">m9 m13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">massAction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diffusion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fixedExchange</t>
   </si>
 </sst>
 </file>
@@ -357,7 +357,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -484,13 +484,13 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="D:F B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -602,7 +602,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -617,13 +617,13 @@
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="D:F"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -708,7 +708,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -723,13 +723,13 @@
   </sheetPr>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="D:F A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -931,7 +931,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -946,13 +946,13 @@
   </sheetPr>
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="D:F A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1252,7 +1252,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1267,19 +1267,19 @@
   </sheetPr>
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="1" sqref="D:F C17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.8137651821862"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.0242914979757"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.9554655870445"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.4210526315789"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="42.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1336,6 +1336,9 @@
       <c r="F2" s="0" t="s">
         <v>24</v>
       </c>
+      <c r="G2" s="0" t="s">
+        <v>33</v>
+      </c>
       <c r="J2" s="0" t="n">
         <v>0</v>
       </c>
@@ -1562,7 +1565,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1577,13 +1580,13 @@
   </sheetPr>
   <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="D:F A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2499,7 +2502,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2514,13 +2517,13 @@
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D:F"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2946,7 +2949,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2961,13 +2964,13 @@
   </sheetPr>
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="D:F B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3172,7 +3175,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3187,13 +3190,13 @@
   </sheetPr>
   <dimension ref="A2:A15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="D:F A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3269,7 +3272,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3284,13 +3287,13 @@
   </sheetPr>
   <dimension ref="A2:A22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="D:F A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3401,7 +3404,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3416,13 +3419,13 @@
   </sheetPr>
   <dimension ref="A2:A22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="D:F A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3533,7 +3536,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3548,13 +3551,13 @@
   </sheetPr>
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="D:F A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3714,7 +3717,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3729,13 +3732,13 @@
   </sheetPr>
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H13" activeCellId="1" sqref="D:F H13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3972,7 +3975,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>